<commit_message>
Updated Members and Manpower
</commit_message>
<xml_diff>
--- a/Table_Generate/manpower.xlsx
+++ b/Table_Generate/manpower.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/17e821e30eeff6db/Desktop/ELL305_work/Documentation_P2/Table_Generate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{AD3CB67E-3F87-403A-841E-3C7EA39BBBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE8EEC40-E414-4E59-B0C6-5265D36C4BC9}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{AD3CB67E-3F87-403A-841E-3C7EA39BBBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81A8B582-A798-4FDF-8DD5-309FDEA8922E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,22 +16,11 @@
     <sheet name="Form responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="137">
   <si>
     <t>Shubham Aggarwal</t>
   </si>
@@ -285,15 +274,9 @@
     <t>Research</t>
   </si>
   <si>
-    <t>Research based work on how to transfer data with minimum internet usage</t>
-  </si>
-  <si>
     <t>2021EE10653</t>
   </si>
   <si>
-    <t>Overleaf, LaTeX, GitHub Actions, pandoc</t>
-  </si>
-  <si>
     <t>Anshul</t>
   </si>
   <si>
@@ -324,12 +307,6 @@
     <t>2021MT10919</t>
   </si>
   <si>
-    <t>7 segment display</t>
-  </si>
-  <si>
-    <t>LCD design, Arduino, triger identifier for bus, hardware design.</t>
-  </si>
-  <si>
     <t>Research on occupancy estimation</t>
   </si>
   <si>
@@ -381,9 +358,6 @@
     <t>Hardware selection</t>
   </si>
   <si>
-    <t>ESP32, networks</t>
-  </si>
-  <si>
     <t>Tanmai Merugu</t>
   </si>
   <si>
@@ -417,9 +391,6 @@
     <t>Research on LoRa wireless comminication</t>
   </si>
   <si>
-    <t>Research, transmission techniques, Receiver hardware</t>
-  </si>
-  <si>
     <t>Arnav Goel</t>
   </si>
   <si>
@@ -436,6 +407,30 @@
   </si>
   <si>
     <t>GitHub, Research on YT</t>
+  </si>
+  <si>
+    <t>Aryan Mishra</t>
+  </si>
+  <si>
+    <t>2021EE10137</t>
+  </si>
+  <si>
+    <t>Research, Transmission techniques, Receiver hardware</t>
+  </si>
+  <si>
+    <t>ESP32, Networks</t>
+  </si>
+  <si>
+    <t>LCD design, Arduino, Trigger identifier for bus, Hardware design.</t>
+  </si>
+  <si>
+    <t>7 Segment Display</t>
+  </si>
+  <si>
+    <t>Overleaf, LaTeX, GitHub Actions, Pandoc</t>
+  </si>
+  <si>
+    <t>Data transfer with minimum internet usage</t>
   </si>
 </sst>
 </file>
@@ -548,6 +543,10 @@
 </file>
 
 <file path=xl/persons/person4.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person5.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -752,11 +751,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D186"/>
+  <dimension ref="A1:D185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -781,7 +780,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>81</v>
       </c>
@@ -862,15 +861,15 @@
         <v>3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="3">
         <v>5</v>
@@ -904,7 +903,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -965,10 +964,10 @@
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C15" s="3">
         <v>5</v>
@@ -979,16 +978,16 @@
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C16" s="3">
         <v>10</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1007,10 +1006,10 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C18" s="3">
         <v>5</v>
@@ -1019,7 +1018,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>45</v>
       </c>
@@ -1058,15 +1057,15 @@
         <v>8</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="C22" s="3">
         <v>5</v>
@@ -1075,7 +1074,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>67</v>
       </c>
@@ -1086,7 +1085,7 @@
         <v>8</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>97</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
@@ -1100,7 +1099,7 @@
         <v>9</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
@@ -1114,10 +1113,10 @@
         <v>8</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>55</v>
       </c>
@@ -1131,7 +1130,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
@@ -1142,7 +1141,7 @@
         <v>8</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
@@ -1175,10 +1174,10 @@
     </row>
     <row r="30" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C30" s="3">
         <v>4</v>
@@ -1189,10 +1188,10 @@
     </row>
     <row r="31" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C31" s="3">
         <v>7</v>
@@ -1206,7 +1205,7 @@
         <v>16</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C32" s="3">
         <v>7</v>
@@ -1240,7 +1239,7 @@
         <v>3</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
@@ -1254,15 +1253,15 @@
         <v>6</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C36" s="3">
         <v>8</v>
@@ -1273,10 +1272,10 @@
     </row>
     <row r="37" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C37" s="3">
         <v>4</v>
@@ -1296,21 +1295,21 @@
         <v>5</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C39" s="3">
         <v>6</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
@@ -1352,7 +1351,7 @@
         <v>5</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
@@ -1371,7 +1370,7 @@
     </row>
     <row r="44" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>19</v>
@@ -1383,7 +1382,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>71</v>
       </c>
@@ -1397,9 +1396,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>15</v>
@@ -1413,30 +1412,30 @@
     </row>
     <row r="47" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C47" s="3">
         <v>5</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C48" s="3">
         <v>9</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
@@ -1469,16 +1468,16 @@
     </row>
     <row r="51" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C51" s="3">
         <v>8</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
@@ -1492,15 +1491,15 @@
         <v>8</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C53" s="3">
         <v>7</v>
@@ -1509,7 +1508,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>17</v>
       </c>
@@ -1523,7 +1522,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>66</v>
       </c>
@@ -1534,7 +1533,7 @@
         <v>6</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1567,23 +1566,31 @@
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C58" s="3">
         <v>4</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="2"/>
+      <c r="A59" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C59" s="3">
+        <v>10</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
@@ -1748,9 +1755,6 @@
       <c r="D86" s="2"/>
     </row>
     <row r="87" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="2"/>
-      <c r="B87" s="2"/>
-      <c r="C87" s="3"/>
       <c r="D87" s="2"/>
     </row>
     <row r="88" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2047,10 +2051,8 @@
     <row r="185" spans="4:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D185" s="2"/>
     </row>
-    <row r="186" spans="4:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D186" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>